<commit_message>
connected web frontend to backend
</commit_message>
<xml_diff>
--- a/rest api - rute.xlsx
+++ b/rest api - rute.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kresica\Desktop\OICAR\OICAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655C12D7-14E0-470D-947F-B2CAE244CD78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15751F5B-7701-4EDE-9EA7-02726D133EEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9480" yWindow="5280" windowWidth="21600" windowHeight="12735" xr2:uid="{74E8284F-5CD1-42BC-BDF1-8223C3917C40}"/>
+    <workbookView xWindow="7200" yWindow="5280" windowWidth="21600" windowHeight="12735" xr2:uid="{74E8284F-5CD1-42BC-BDF1-8223C3917C40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>api/restaurant/destkop/reg</t>
   </si>
@@ -68,9 +68,6 @@
     <t>IZGLED OBJEKTA:</t>
   </si>
   <si>
-    <t>api/restaurant/web/view</t>
-  </si>
-  <si>
     <t>string username , string pass, string email</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
   </si>
   <si>
     <t>WebUser</t>
-  </si>
-  <si>
-    <t>string detalji restorana,string[] hrana, string[] vina,doble ocjena, Bitmap image</t>
   </si>
   <si>
     <t>posta registraciju web usera</t>
@@ -142,6 +136,18 @@
   </si>
   <si>
     <t>posta vina za odredeni restoran</t>
+  </si>
+  <si>
+    <t>string imeRestorana, string detalji restorana,string[] hrana, string[] vina,doble ocjena, Bitmap image</t>
+  </si>
+  <si>
+    <t>api/restaurant/destkop/login</t>
+  </si>
+  <si>
+    <t>vraca detalje restaurantOwnera</t>
+  </si>
+  <si>
+    <t>api/restaurant/web/login</t>
   </si>
 </sst>
 </file>
@@ -491,9 +497,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -535,6 +538,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -852,7 +858,7 @@
   <dimension ref="B1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,7 +867,7 @@
     <col min="3" max="3" width="39.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="76" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="96.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="39.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.85546875" customWidth="1"/>
     <col min="9" max="9" width="22.7109375" customWidth="1"/>
@@ -869,173 +875,177 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="12"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="13" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="14" t="s">
+      <c r="E2" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="24" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="D3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="18"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="18"/>
-      <c r="C5" s="21" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="24"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="17"/>
+      <c r="C6" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="E6" s="24"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="33"/>
+      <c r="C7" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="18"/>
-      <c r="C6" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-    </row>
-    <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="34"/>
-      <c r="C7" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="35"/>
-      <c r="F7" s="37"/>
-    </row>
-    <row r="8" spans="2:12" ht="24" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="5" t="s">
+      <c r="E7" s="34"/>
+      <c r="F7" s="36"/>
+    </row>
+    <row r="8" spans="2:12" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="7"/>
+      <c r="C8" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C9" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="32" t="s">
+      <c r="D9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="33" t="s">
+      <c r="E9" s="25"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="7"/>
+      <c r="C10" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="25"/>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="7"/>
+      <c r="C11" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="25"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="8"/>
+      <c r="C12" s="22" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
-      <c r="C9" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="26"/>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
-      <c r="C11" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="26"/>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="9"/>
-      <c r="C12" s="23" t="s">
+      <c r="D12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="27"/>
-      <c r="F12" s="11"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="10"/>
     </row>
     <row r="14" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
connected desktop app to backend
</commit_message>
<xml_diff>
--- a/rest api - rute.xlsx
+++ b/rest api - rute.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kresica\Desktop\OICAR\OICAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15751F5B-7701-4EDE-9EA7-02726D133EEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3457BA76-6BD2-4F81-96B7-EAB07016593E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="5280" windowWidth="21600" windowHeight="12735" xr2:uid="{74E8284F-5CD1-42BC-BDF1-8223C3917C40}"/>
+    <workbookView xWindow="-24765" yWindow="5175" windowWidth="21600" windowHeight="12735" xr2:uid="{74E8284F-5CD1-42BC-BDF1-8223C3917C40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -95,6 +95,33 @@
     <t>posta registraciju desktop usera</t>
   </si>
   <si>
+    <t>api/restaurant/desktop/img</t>
+  </si>
+  <si>
+    <t>api/restaurant/desktop/food</t>
+  </si>
+  <si>
+    <t>posta hranu za odredeni restoran</t>
+  </si>
+  <si>
+    <t>posta sliku za odredeni restoran</t>
+  </si>
+  <si>
+    <t>api/restaurant/desktop/wine</t>
+  </si>
+  <si>
+    <t>posta vina za odredeni restoran</t>
+  </si>
+  <si>
+    <t>api/restaurant/destkop/login</t>
+  </si>
+  <si>
+    <t>vraca detalje restaurantOwnera</t>
+  </si>
+  <si>
+    <t>api/restaurant/web/login</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">string username , string pass, </t>
     </r>
@@ -116,38 +143,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> restoran</t>
+      <t xml:space="preserve"> restaurant</t>
     </r>
   </si>
   <si>
-    <t>api/restaurant/desktop/img</t>
-  </si>
-  <si>
-    <t>api/restaurant/desktop/food</t>
-  </si>
-  <si>
-    <t>posta hranu za odredeni restoran</t>
-  </si>
-  <si>
-    <t>posta sliku za odredeni restoran</t>
-  </si>
-  <si>
-    <t>api/restaurant/desktop/wine</t>
-  </si>
-  <si>
-    <t>posta vina za odredeni restoran</t>
-  </si>
-  <si>
-    <t>string imeRestorana, string detalji restorana,string[] hrana, string[] vina,doble ocjena, Bitmap image</t>
-  </si>
-  <si>
-    <t>api/restaurant/destkop/login</t>
-  </si>
-  <si>
-    <t>vraca detalje restaurantOwnera</t>
-  </si>
-  <si>
-    <t>api/restaurant/web/login</t>
+    <t>string RestaurantName, string RestaurantDetails,string Food, string wine,doble Grade, string Image</t>
   </si>
 </sst>
 </file>
@@ -858,7 +858,7 @@
   <dimension ref="B1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,7 +901,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -912,16 +912,16 @@
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="17"/>
       <c r="C4" s="20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E4" s="29" t="s">
         <v>15</v>
       </c>
       <c r="F4" s="30" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -933,10 +933,10 @@
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="17"/>
       <c r="C5" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="24"/>
       <c r="F5" s="16"/>
@@ -950,10 +950,10 @@
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="17"/>
       <c r="C6" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="15" t="s">
         <v>22</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>23</v>
       </c>
       <c r="E6" s="24"/>
       <c r="F6" s="16"/>
@@ -967,10 +967,10 @@
     <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="33"/>
       <c r="C7" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="35" t="s">
         <v>25</v>
-      </c>
-      <c r="D7" s="35" t="s">
-        <v>26</v>
       </c>
       <c r="E7" s="34"/>
       <c r="F7" s="36"/>
@@ -978,7 +978,7 @@
     <row r="8" spans="2:12" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7"/>
       <c r="C8" s="21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added Multiple Language support and animations
</commit_message>
<xml_diff>
--- a/rest api - rute.xlsx
+++ b/rest api - rute.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kresica\Desktop\OICAR\OICAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3457BA76-6BD2-4F81-96B7-EAB07016593E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149322E0-1B8C-443E-9D9D-07BA5149A95A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24765" yWindow="5175" windowWidth="21600" windowHeight="12735" xr2:uid="{74E8284F-5CD1-42BC-BDF1-8223C3917C40}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{74E8284F-5CD1-42BC-BDF1-8223C3917C40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>api/restaurant/destkop/reg</t>
   </si>
@@ -147,14 +147,113 @@
     </r>
   </si>
   <si>
-    <t>string RestaurantName, string RestaurantDetails,string Food, string wine,doble Grade, string Image</t>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Wine</t>
+  </si>
+  <si>
+    <t>GradeSpread</t>
+  </si>
+  <si>
+    <t>int One, int Two, int Three, int Four, int Five</t>
+  </si>
+  <si>
+    <r>
+      <t>string RestaurantName, string RestaurantDetails,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Food</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Food, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Wine</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Wine, string Image, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GradeSpread</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  Grade</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">string Name, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">GradeSpread </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Grade, double Price,string Image</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,8 +284,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,8 +311,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -476,21 +587,67 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thick">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -511,9 +668,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -521,7 +675,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
@@ -537,12 +690,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -855,10 +1015,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71D6FEA-AA44-4C63-8BF0-121472999A15}">
-  <dimension ref="B1:L15"/>
+  <dimension ref="B1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -867,7 +1027,7 @@
     <col min="3" max="3" width="39.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="96.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="98.28515625" customWidth="1"/>
     <col min="7" max="7" width="39.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.85546875" customWidth="1"/>
     <col min="9" max="9" width="22.7109375" customWidth="1"/>
@@ -876,11 +1036,11 @@
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11"/>
-      <c r="C2" s="18"/>
+      <c r="C2" s="17"/>
       <c r="D2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="22" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="13" t="s">
@@ -891,16 +1051,16 @@
       <c r="B3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="18" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="26" t="s">
         <v>29</v>
       </c>
       <c r="G3" s="3"/>
@@ -910,18 +1070,18 @@
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="17"/>
-      <c r="C4" s="20" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="19" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="30" t="s">
-        <v>30</v>
+      <c r="F4" s="35" t="s">
+        <v>34</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -931,15 +1091,15 @@
       <c r="L4" s="3"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="17"/>
-      <c r="C5" s="20" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="16"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="36"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -948,15 +1108,19 @@
       <c r="L5" s="3"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="17"/>
-      <c r="C6" s="20" t="s">
+      <c r="B6" s="16"/>
+      <c r="C6" s="19" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="16"/>
+      <c r="E6" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>35</v>
+      </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -964,93 +1128,114 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="33"/>
-      <c r="C7" s="34" t="s">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="16"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="31"/>
+      <c r="C8" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D8" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="36"/>
-    </row>
-    <row r="8" spans="2:12" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="7"/>
-      <c r="C8" s="21" t="s">
+      <c r="E8" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="7"/>
+      <c r="C9" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E9" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F9" s="30" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B9" s="4" t="s">
+    <row r="10" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B10" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C10" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
-      <c r="C10" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="25"/>
+      <c r="E10" s="23"/>
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="23"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="7"/>
+      <c r="C12" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="8"/>
-      <c r="C12" s="22" t="s">
+      <c r="E12" s="23"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="8"/>
+      <c r="C13" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="26"/>
-      <c r="F12" s="10"/>
-    </row>
-    <row r="14" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B14" s="1"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="10"/>
+    </row>
+    <row r="15" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B15" s="1"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C14:E14"/>
     <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated web api ui
</commit_message>
<xml_diff>
--- a/rest api - rute.xlsx
+++ b/rest api - rute.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kresica\Desktop\OICAR\OICAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DCED187-2549-43DC-A25C-8BFCDD231409}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387AE9ED-CAD2-4F67-A096-615F2269D9F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6135" yWindow="2985" windowWidth="21600" windowHeight="12735" xr2:uid="{74E8284F-5CD1-42BC-BDF1-8223C3917C40}"/>
   </bookViews>
@@ -252,7 +252,7 @@
     <t>api/restaurant/web/gradespread/update</t>
   </si>
   <si>
-    <t xml:space="preserve">posta update I vraca listu restorana </t>
+    <t xml:space="preserve">posta restaurant model I vraca listu restorana </t>
   </si>
 </sst>
 </file>
@@ -1024,7 +1024,7 @@
   <dimension ref="B1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C16" sqref="C16:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>